<commit_message>
Added more attributes to the data model, including corresponding reference data. Still much more to be added.
</commit_message>
<xml_diff>
--- a/seeddata-bsdf/99-exceldmd/PIM2.0v5 - Reference Data Model.xlsx
+++ b/seeddata-bsdf/99-exceldmd/PIM2.0v5 - Reference Data Model.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikhilbhatia/github/customer-seed-bsdf/99-exceldmd/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\a\git\Beiersdorf\seeddata-bsdf\99-exceldmd\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="38320" windowHeight="23540" tabRatio="544" activeTab="6"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="38325" windowHeight="23535" tabRatio="544"/>
   </bookViews>
   <sheets>
     <sheet name="HELP" sheetId="1" r:id="rId1"/>
@@ -38,8 +38,8 @@
   </definedNames>
   <calcPr calcId="145621" iterateDelta="1E-4" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1676" windowHeight="854" tabRatio="500" activeSheetId="7"/>
     <customWorkbookView name="Gupta, Kunal - Personal View" guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1360" windowHeight="539" tabRatio="500" activeSheetId="7"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1676" windowHeight="854" tabRatio="500" activeSheetId="7"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -58,7 +58,7 @@
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="348">
   <si>
     <t>ACTION</t>
   </si>
@@ -441,36 +441,6 @@
     <t>Thick hair</t>
   </si>
   <si>
-    <t>ht00</t>
-  </si>
-  <si>
-    <t>ht01</t>
-  </si>
-  <si>
-    <t>ht02</t>
-  </si>
-  <si>
-    <t>ht03</t>
-  </si>
-  <si>
-    <t>ht04</t>
-  </si>
-  <si>
-    <t>ht05</t>
-  </si>
-  <si>
-    <t>ht06</t>
-  </si>
-  <si>
-    <t>ht07</t>
-  </si>
-  <si>
-    <t>ht08</t>
-  </si>
-  <si>
-    <t>ht09</t>
-  </si>
-  <si>
     <t>/~/images/mam/-120391-1.png</t>
   </si>
   <si>
@@ -492,12 +462,6 @@
     <t>Critical</t>
   </si>
   <si>
-    <t>c0</t>
-  </si>
-  <si>
-    <t>c1</t>
-  </si>
-  <si>
     <t>Attribute 6</t>
   </si>
   <si>
@@ -585,24 +549,6 @@
     <t>Body - Hand Cream &amp; Soap</t>
   </si>
   <si>
-    <t>tn0101</t>
-  </si>
-  <si>
-    <t>tn0102</t>
-  </si>
-  <si>
-    <t>tn0103</t>
-  </si>
-  <si>
-    <t>tn0201</t>
-  </si>
-  <si>
-    <t>tn0202</t>
-  </si>
-  <si>
-    <t>tn0203</t>
-  </si>
-  <si>
     <t>Baby/Kids - Care (Baby)</t>
   </si>
   <si>
@@ -612,69 +558,36 @@
     <t>Baby/Kids - Suncare (Baby)</t>
   </si>
   <si>
-    <t>tn0301</t>
-  </si>
-  <si>
     <t>Face - Cleansers &amp; Toners</t>
   </si>
   <si>
-    <t>tr01</t>
-  </si>
-  <si>
     <t>After Shave</t>
   </si>
   <si>
-    <t>tr02</t>
-  </si>
-  <si>
     <t>Baby</t>
   </si>
   <si>
-    <t>tr03</t>
-  </si>
-  <si>
     <t>Bath Care</t>
   </si>
   <si>
-    <t>tr04</t>
-  </si>
-  <si>
     <t>Deo</t>
   </si>
   <si>
-    <t>tr05</t>
-  </si>
-  <si>
     <t>Depillatories</t>
   </si>
   <si>
-    <t>tr06</t>
-  </si>
-  <si>
     <t>Face Care</t>
   </si>
   <si>
-    <t>tr07</t>
-  </si>
-  <si>
     <t>Foot Care</t>
   </si>
   <si>
-    <t>tr08</t>
-  </si>
-  <si>
     <t>Hair Care</t>
   </si>
   <si>
-    <t>tr09</t>
-  </si>
-  <si>
     <t>Hairstyling</t>
   </si>
   <si>
-    <t>tr10</t>
-  </si>
-  <si>
     <t>Lip Care</t>
   </si>
   <si>
@@ -1054,12 +967,180 @@
   </si>
   <si>
     <t>Draft</t>
+  </si>
+  <si>
+    <t>dgender</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>dpvregions</t>
+  </si>
+  <si>
+    <t>PV Regions</t>
+  </si>
+  <si>
+    <t>Gender Key</t>
+  </si>
+  <si>
+    <t>Gender Label</t>
+  </si>
+  <si>
+    <t>PV Region Key</t>
+  </si>
+  <si>
+    <t>PV Region Label</t>
+  </si>
+  <si>
+    <t>Women</t>
+  </si>
+  <si>
+    <t>Men</t>
+  </si>
+  <si>
+    <t>Unisex</t>
+  </si>
+  <si>
+    <t>Kids</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>Americas</t>
+  </si>
+  <si>
+    <t>Near East</t>
+  </si>
+  <si>
+    <t>CEE</t>
+  </si>
+  <si>
+    <t>zg01</t>
+  </si>
+  <si>
+    <t>zg02</t>
+  </si>
+  <si>
+    <t>zg03</t>
+  </si>
+  <si>
+    <t>zg04</t>
+  </si>
+  <si>
+    <t>zg05</t>
+  </si>
+  <si>
+    <t>zpvr01</t>
+  </si>
+  <si>
+    <t>zpvr02</t>
+  </si>
+  <si>
+    <t>zpvr03</t>
+  </si>
+  <si>
+    <t>zpvr04</t>
+  </si>
+  <si>
+    <t>ztr10</t>
+  </si>
+  <si>
+    <t>zc0</t>
+  </si>
+  <si>
+    <t>zc1</t>
+  </si>
+  <si>
+    <t>zht00</t>
+  </si>
+  <si>
+    <t>zht01</t>
+  </si>
+  <si>
+    <t>zht02</t>
+  </si>
+  <si>
+    <t>zht03</t>
+  </si>
+  <si>
+    <t>zht04</t>
+  </si>
+  <si>
+    <t>zht05</t>
+  </si>
+  <si>
+    <t>zht06</t>
+  </si>
+  <si>
+    <t>zht07</t>
+  </si>
+  <si>
+    <t>zht08</t>
+  </si>
+  <si>
+    <t>zht09</t>
+  </si>
+  <si>
+    <t>ztn0101</t>
+  </si>
+  <si>
+    <t>ztn0102</t>
+  </si>
+  <si>
+    <t>ztn0103</t>
+  </si>
+  <si>
+    <t>ztn0201</t>
+  </si>
+  <si>
+    <t>ztn0202</t>
+  </si>
+  <si>
+    <t>ztn0203</t>
+  </si>
+  <si>
+    <t>ztn0301</t>
+  </si>
+  <si>
+    <t>ztr01</t>
+  </si>
+  <si>
+    <t>ztr02</t>
+  </si>
+  <si>
+    <t>ztr03</t>
+  </si>
+  <si>
+    <t>ztr04</t>
+  </si>
+  <si>
+    <t>ztr05</t>
+  </si>
+  <si>
+    <t>ztr06</t>
+  </si>
+  <si>
+    <t>ztr07</t>
+  </si>
+  <si>
+    <t>ztr08</t>
+  </si>
+  <si>
+    <t>ztr09</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>reference data key values, used to clearly define what is simply "data" and what is not (values starting with c are expected to be Contexts)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]General"/>
   </numFmts>
@@ -1268,7 +1349,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1316,6 +1397,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Excel Built-in Normal" xfId="3"/>
@@ -1644,18 +1726,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:C34"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" customWidth="1"/>
-    <col min="3" max="3" width="90.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.125" customWidth="1"/>
+    <col min="3" max="3" width="90.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1717,7 +1799,7 @@
         <v>94</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>5</v>
@@ -1725,10 +1807,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
-        <v>204</v>
+        <v>175</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C21" s="31" t="s">
         <v>76</v>
@@ -1736,10 +1818,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
-        <v>205</v>
+        <v>176</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C22" s="31" t="s">
         <v>95</v>
@@ -1747,10 +1829,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
-        <v>206</v>
+        <v>177</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C23" s="31" t="s">
         <v>96</v>
@@ -1758,10 +1840,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C24" s="31" t="s">
         <v>97</v>
@@ -1769,10 +1851,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
-        <v>208</v>
+        <v>179</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C25" s="31" t="s">
         <v>98</v>
@@ -1780,21 +1862,21 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="30" t="s">
-        <v>209</v>
+        <v>180</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="30" t="s">
-        <v>210</v>
+        <v>181</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="C27" s="31" t="s">
         <v>99</v>
@@ -1802,10 +1884,10 @@
     </row>
     <row r="28" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="B28" s="31" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="C28" s="31" t="s">
         <v>103</v>
@@ -1813,21 +1895,21 @@
     </row>
     <row r="29" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="30" t="s">
-        <v>254</v>
+        <v>225</v>
       </c>
       <c r="B29" s="31" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>255</v>
+        <v>226</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="30" t="s">
-        <v>212</v>
+        <v>183</v>
       </c>
       <c r="B30" s="31" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="C30" s="31" t="s">
         <v>100</v>
@@ -1835,55 +1917,66 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
-        <v>213</v>
+        <v>184</v>
       </c>
       <c r="B31" s="31" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
-        <v>214</v>
+        <v>185</v>
       </c>
       <c r="B32" s="31" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="30" t="s">
-        <v>215</v>
+        <v>186</v>
       </c>
       <c r="B33" s="31" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
-        <v>216</v>
+        <v>187</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>160</v>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="30" t="s">
+        <v>346</v>
+      </c>
+      <c r="B36" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="C36" t="s">
+        <v>347</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="150">
+    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="150">
       <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="150">
+    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="150">
       <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -1902,21 +1995,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A4:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2053,11 +2146,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="139">
+    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="139">
       <selection activeCell="E22" sqref="E22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="139">
+    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="139">
       <selection activeCell="E22" sqref="E22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -2069,22 +2162,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:D9"/>
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="27.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2098,82 +2191,98 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>217</v>
+        <v>188</v>
       </c>
       <c r="C2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="C3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>219</v>
+        <v>190</v>
       </c>
       <c r="C4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>220</v>
+        <v>191</v>
       </c>
       <c r="C5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>221</v>
+        <v>192</v>
       </c>
       <c r="C6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B7" s="29" t="s">
-        <v>222</v>
+        <v>193</v>
       </c>
       <c r="C7" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>303</v>
+        <v>274</v>
       </c>
       <c r="C8" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>230</v>
+        <v>201</v>
       </c>
       <c r="C9" t="s">
-        <v>151</v>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="29" t="s">
+        <v>294</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1"/>
   <customSheetViews>
+    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="125" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:D1194"/>
+    </customSheetView>
     <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="125" showAutoFilter="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:D1194"/>
-    </customSheetView>
-    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="125" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="A1:D1194"/>
     </customSheetView>
@@ -2184,37 +2293,37 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8:B9"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2273,9 +2382,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B2" s="29" t="s">
-        <v>223</v>
+        <v>194</v>
       </c>
       <c r="C2" t="s">
         <v>86</v>
@@ -2296,9 +2405,9 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>224</v>
+        <v>195</v>
       </c>
       <c r="C3" t="s">
         <v>86</v>
@@ -2319,77 +2428,77 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>225</v>
+        <v>196</v>
       </c>
       <c r="C4" t="s">
         <v>86</v>
       </c>
       <c r="E4" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F4" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="G4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>226</v>
+        <v>197</v>
       </c>
       <c r="C5" t="s">
         <v>86</v>
       </c>
       <c r="E5" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F5" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="G5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>227</v>
+        <v>198</v>
       </c>
       <c r="C6" t="s">
         <v>86</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F6" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="G6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>228</v>
+        <v>199</v>
       </c>
       <c r="C7" t="s">
         <v>86</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F7" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="G7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>305</v>
+        <v>276</v>
       </c>
       <c r="C8" t="s">
         <v>86</v>
@@ -2398,15 +2507,15 @@
         <v>99</v>
       </c>
       <c r="F8" t="s">
-        <v>307</v>
+        <v>278</v>
       </c>
       <c r="G8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>306</v>
+        <v>277</v>
       </c>
       <c r="C9" t="s">
         <v>86</v>
@@ -2415,7 +2524,7 @@
         <v>99</v>
       </c>
       <c r="F9" t="s">
-        <v>308</v>
+        <v>279</v>
       </c>
       <c r="G9" t="s">
         <v>31</v>
@@ -2424,19 +2533,19 @@
   </sheetData>
   <autoFilter ref="A1:S1"/>
   <customSheetViews>
+    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="93" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+      <autoFilter ref="A1:S43"/>
+    </customSheetView>
     <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="93" showAutoFilter="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
       <autoFilter ref="A1:S35"/>
-    </customSheetView>
-    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="93" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-      <autoFilter ref="A1:S43"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2446,28 +2555,28 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0"/>
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.125" customWidth="1"/>
+    <col min="4" max="4" width="16.375" customWidth="1"/>
+    <col min="5" max="5" width="16.625" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="10" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.125" customWidth="1"/>
+    <col min="8" max="8" width="16.625" customWidth="1"/>
+    <col min="9" max="9" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2499,21 +2608,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>229</v>
+        <v>200</v>
       </c>
       <c r="C2" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="D2" t="s">
-        <v>230</v>
+        <v>201</v>
       </c>
       <c r="E2" t="s">
-        <v>220</v>
+        <v>191</v>
       </c>
       <c r="H2" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -2521,11 +2630,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="107">
+    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="107">
       <selection activeCell="G10" sqref="G10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="107">
+    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="107">
       <selection activeCell="G10" sqref="G10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -2537,35 +2646,35 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet6" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:P22"/>
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.83203125" customWidth="1"/>
-    <col min="4" max="4" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.875" customWidth="1"/>
+    <col min="4" max="4" width="29.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.5" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" customWidth="1"/>
-    <col min="10" max="10" width="21.83203125" customWidth="1"/>
-    <col min="11" max="11" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.625" customWidth="1"/>
+    <col min="10" max="10" width="21.875" customWidth="1"/>
+    <col min="11" max="11" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.375" customWidth="1"/>
     <col min="13" max="13" width="17.5" customWidth="1"/>
-    <col min="14" max="14" width="19.1640625" customWidth="1"/>
+    <col min="14" max="14" width="19.125" customWidth="1"/>
     <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2615,12 +2724,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>217</v>
+        <v>188</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>223</v>
+        <v>194</v>
       </c>
       <c r="E2" s="29"/>
       <c r="F2" s="29" t="s">
@@ -2643,12 +2752,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B3" s="29" t="s">
-        <v>217</v>
+        <v>188</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>224</v>
+        <v>195</v>
       </c>
       <c r="E3" s="29"/>
       <c r="F3" s="29"/>
@@ -2671,12 +2780,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>223</v>
+        <v>194</v>
       </c>
       <c r="F4" t="s">
         <v>30</v>
@@ -2691,12 +2800,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B5" s="29" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>224</v>
+        <v>195</v>
       </c>
       <c r="G5" t="s">
         <v>30</v>
@@ -2711,74 +2820,74 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B6" s="29" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>225</v>
+        <v>196</v>
       </c>
       <c r="K6" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="P6" s="29" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B7" s="29" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>226</v>
+        <v>197</v>
       </c>
       <c r="K7" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="P7" s="29" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B8" s="29" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>227</v>
+        <v>198</v>
       </c>
       <c r="K8" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="P8" s="29" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B9" s="29" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>228</v>
+        <v>199</v>
       </c>
       <c r="K9" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="P9" s="29" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B10" s="29" t="s">
-        <v>219</v>
+        <v>190</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>223</v>
+        <v>194</v>
       </c>
       <c r="F10" s="29" t="s">
         <v>30</v>
       </c>
       <c r="K10" s="29" t="s">
-        <v>202</v>
+        <v>173</v>
       </c>
       <c r="M10" s="29" t="s">
         <v>30</v>
@@ -2787,18 +2896,18 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B11" s="29" t="s">
-        <v>219</v>
+        <v>190</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>224</v>
+        <v>195</v>
       </c>
       <c r="G11" s="29" t="s">
         <v>30</v>
       </c>
       <c r="K11" s="29" t="s">
-        <v>203</v>
+        <v>174</v>
       </c>
       <c r="M11" s="29" t="s">
         <v>30</v>
@@ -2807,12 +2916,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>220</v>
+        <v>191</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>223</v>
+        <v>194</v>
       </c>
       <c r="E12" s="29"/>
       <c r="F12" s="29" t="s">
@@ -2823,7 +2932,7 @@
       <c r="I12" s="29"/>
       <c r="J12" s="29"/>
       <c r="K12" s="29" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="L12" s="29"/>
       <c r="M12" s="29" t="s">
@@ -2835,12 +2944,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B13" s="29" t="s">
-        <v>220</v>
+        <v>191</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>224</v>
+        <v>195</v>
       </c>
       <c r="E13" s="29"/>
       <c r="F13" s="29"/>
@@ -2851,7 +2960,7 @@
       <c r="I13" s="29"/>
       <c r="J13" s="29"/>
       <c r="K13" s="29" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="L13" s="29"/>
       <c r="M13" s="29" t="s">
@@ -2863,12 +2972,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>230</v>
+        <v>201</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>223</v>
+        <v>194</v>
       </c>
       <c r="E14" s="29"/>
       <c r="F14" s="29" t="s">
@@ -2879,7 +2988,7 @@
       <c r="I14" s="29"/>
       <c r="J14" s="29"/>
       <c r="K14" s="29" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="L14" s="29"/>
       <c r="M14" s="29" t="s">
@@ -2891,12 +3000,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B15" s="29" t="s">
-        <v>230</v>
+        <v>201</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>224</v>
+        <v>195</v>
       </c>
       <c r="E15" s="29"/>
       <c r="F15" s="29"/>
@@ -2907,7 +3016,7 @@
       <c r="I15" s="29"/>
       <c r="J15" s="29"/>
       <c r="K15" s="29" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="L15" s="29"/>
       <c r="M15" s="29" t="s">
@@ -2919,32 +3028,32 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B16" s="29" t="s">
-        <v>230</v>
+        <v>201</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>229</v>
+        <v>200</v>
       </c>
       <c r="K16" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="P16" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>221</v>
+        <v>192</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>223</v>
+        <v>194</v>
       </c>
       <c r="F17" t="s">
         <v>30</v>
       </c>
       <c r="K17" t="s">
-        <v>197</v>
+        <v>168</v>
       </c>
       <c r="M17" t="s">
         <v>30</v>
@@ -2953,18 +3062,18 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B18" s="29" t="s">
-        <v>221</v>
+        <v>192</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>224</v>
+        <v>195</v>
       </c>
       <c r="G18" t="s">
         <v>30</v>
       </c>
       <c r="K18" t="s">
-        <v>198</v>
+        <v>169</v>
       </c>
       <c r="M18" t="s">
         <v>30</v>
@@ -2973,18 +3082,18 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="2:16" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B19" s="29" t="s">
-        <v>222</v>
+        <v>193</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>223</v>
+        <v>194</v>
       </c>
       <c r="F19" s="29" t="s">
         <v>30</v>
       </c>
       <c r="K19" s="29" t="s">
-        <v>199</v>
+        <v>170</v>
       </c>
       <c r="M19" s="29" t="s">
         <v>30</v>
@@ -2993,18 +3102,18 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="2:16" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B20" s="29" t="s">
-        <v>222</v>
+        <v>193</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>224</v>
+        <v>195</v>
       </c>
       <c r="G20" s="29" t="s">
         <v>30</v>
       </c>
       <c r="K20" s="29" t="s">
-        <v>200</v>
+        <v>171</v>
       </c>
       <c r="M20" s="29" t="s">
         <v>30</v>
@@ -3013,12 +3122,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>303</v>
+        <v>274</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>305</v>
+        <v>276</v>
       </c>
       <c r="G21" t="s">
         <v>30</v>
@@ -3027,18 +3136,134 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>303</v>
+        <v>274</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>306</v>
+        <v>277</v>
       </c>
       <c r="F22" t="s">
         <v>30</v>
       </c>
       <c r="P22" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B23" s="29" t="s">
+        <v>292</v>
+      </c>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29" t="s">
+        <v>296</v>
+      </c>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="N23" s="29"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B24" s="29" t="s">
+        <v>292</v>
+      </c>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29" t="s">
+        <v>297</v>
+      </c>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="N24" s="29"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B25" s="29" t="s">
+        <v>294</v>
+      </c>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29" t="s">
+        <v>298</v>
+      </c>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="N25" s="29"/>
+      <c r="O25" s="29"/>
+      <c r="P25" s="29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B26" s="29" t="s">
+        <v>294</v>
+      </c>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="L26" s="29"/>
+      <c r="M26" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="N26" s="29"/>
+      <c r="O26" s="29"/>
+      <c r="P26" s="29" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -3047,19 +3272,19 @@
     <sortCondition ref="B1"/>
   </sortState>
   <customSheetViews>
+    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="90" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+      <autoFilter ref="A1:P2402"/>
+    </customSheetView>
     <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="90" showAutoFilter="1">
       <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId1"/>
+      <pageSetup orientation="portrait" r:id="rId2"/>
       <autoFilter ref="A1:P2390"/>
-    </customSheetView>
-    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="90" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="A1:P2402"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3069,36 +3294,36 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet7" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:U81"/>
+  <sheetPr codeName="Sheet7"/>
+  <dimension ref="A1:U90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="H81" sqref="H81"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" style="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" style="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.625" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.875" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.625" style="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.625" style="29" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.1640625" style="28" customWidth="1"/>
-    <col min="8" max="8" width="35.6640625" style="28" customWidth="1"/>
+    <col min="7" max="7" width="26.125" style="28" customWidth="1"/>
+    <col min="8" max="8" width="35.625" style="28" customWidth="1"/>
     <col min="9" max="9" width="23.5" style="28" customWidth="1"/>
-    <col min="10" max="10" width="23.6640625" style="28" customWidth="1"/>
-    <col min="11" max="11" width="68.33203125" style="29" customWidth="1"/>
-    <col min="12" max="12" width="31.6640625" style="29" customWidth="1"/>
-    <col min="13" max="15" width="14.1640625" style="29" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.1640625" style="29" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.1640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.625" style="28" customWidth="1"/>
+    <col min="11" max="11" width="68.375" style="29" customWidth="1"/>
+    <col min="12" max="12" width="31.625" style="29" customWidth="1"/>
+    <col min="13" max="15" width="14.125" style="29" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.125" style="29" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.125" style="29" bestFit="1" customWidth="1"/>
     <col min="18" max="21" width="17" style="29" bestFit="1" customWidth="1"/>
     <col min="22" max="16384" width="11" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3163,1081 +3388,1180 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B2" s="29" t="s">
-        <v>217</v>
+        <v>188</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>133</v>
+        <v>318</v>
       </c>
       <c r="H2" s="28" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B3" s="29" t="s">
-        <v>217</v>
+        <v>188</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>134</v>
+        <v>319</v>
       </c>
       <c r="H3" s="28" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B4" s="29" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>116</v>
+        <v>320</v>
       </c>
       <c r="H4" s="28" t="s">
         <v>106</v>
       </c>
       <c r="I4" s="28" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="J4" s="28" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="K4" s="29" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="L4" s="28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B5" s="29" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>117</v>
+        <v>321</v>
       </c>
       <c r="H5" s="28" t="s">
         <v>113</v>
       </c>
       <c r="I5" s="28" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="J5" s="28" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="K5" s="29" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="L5" s="28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B6" s="29" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>118</v>
+        <v>322</v>
       </c>
       <c r="H6" s="28" t="s">
         <v>107</v>
       </c>
       <c r="I6" s="28" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="J6" s="28" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="K6" s="29" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="L6" s="28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B7" s="29" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>119</v>
+        <v>323</v>
       </c>
       <c r="H7" s="28" t="s">
         <v>108</v>
       </c>
       <c r="I7" s="28" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="J7" s="28" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="K7" s="29" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="L7" s="28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B8" s="29" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>120</v>
+        <v>324</v>
       </c>
       <c r="H8" s="28" t="s">
         <v>109</v>
       </c>
       <c r="I8" s="28" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="J8" s="28" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="K8" s="29" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="L8" s="28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B9" s="29" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>121</v>
+        <v>325</v>
       </c>
       <c r="H9" s="28" t="s">
         <v>110</v>
       </c>
       <c r="I9" s="28" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="J9" s="28" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="K9" s="29" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="L9" s="28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B10" s="29" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>122</v>
+        <v>326</v>
       </c>
       <c r="H10" s="28" t="s">
         <v>111</v>
       </c>
       <c r="I10" s="28" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="J10" s="28" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="K10" s="29" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="L10" s="28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B11" s="29" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>123</v>
+        <v>327</v>
       </c>
       <c r="H11" s="28" t="s">
         <v>112</v>
       </c>
       <c r="I11" s="28" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="J11" s="28" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="K11" s="29" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="L11" s="28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B12" s="29" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>124</v>
+        <v>328</v>
       </c>
       <c r="H12" s="28" t="s">
         <v>114</v>
       </c>
       <c r="I12" s="28" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="J12" s="28" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="K12" s="29" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="L12" s="28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B13" s="29" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>125</v>
+        <v>329</v>
       </c>
       <c r="H13" s="28" t="s">
         <v>115</v>
       </c>
       <c r="I13" s="28" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="J13" s="28" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="K13" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="L13" s="28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B14" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="G14" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="H14" s="29" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B15" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="G15" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="H15" s="29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B16" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="G16" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="H16" s="29" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B17" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="G17" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B18" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="G18" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="H18" s="29" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B19" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="G19" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="H19" s="29" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B20" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="G20" s="29" t="s">
+        <v>213</v>
+      </c>
+      <c r="H20" s="29" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B21" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G21" s="29" t="s">
+        <v>229</v>
+      </c>
+      <c r="H21" s="29" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B22" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G22" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="H22" s="29" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B23" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G23" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="H23" s="29" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B24" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G24" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="H24" s="29" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B25" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G25" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="H25" s="29" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B26" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G26" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="H26" s="29" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B27" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G27" s="29" t="s">
+        <v>233</v>
+      </c>
+      <c r="H27" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B28" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G28" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="H28" s="29" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B29" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G29" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="H29" s="29" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B30" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G30" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="H30" s="29" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B31" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G31" s="29" t="s">
+        <v>237</v>
+      </c>
+      <c r="H31" s="29" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B32" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G32" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="H32" s="29" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B33" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G33" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="H33" s="29" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B34" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G34" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="H34" s="29" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B35" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G35" s="29" t="s">
+        <v>239</v>
+      </c>
+      <c r="H35" s="29" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B36" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G36" s="29" t="s">
+        <v>215</v>
+      </c>
+      <c r="H36" s="29" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B37" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G37" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="H37" s="29" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B38" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G38" s="29" t="s">
+        <v>240</v>
+      </c>
+      <c r="H38" s="29" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B39" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G39" s="29" t="s">
+        <v>241</v>
+      </c>
+      <c r="H39" s="29" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B40" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G40" s="29" t="s">
+        <v>242</v>
+      </c>
+      <c r="H40" s="29" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B41" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G41" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="H41" s="29" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B42" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G42" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="H42" s="29" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B43" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G43" s="29" t="s">
+        <v>245</v>
+      </c>
+      <c r="H43" s="29" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B44" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G44" s="29" t="s">
+        <v>246</v>
+      </c>
+      <c r="H44" s="29" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B45" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G45" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="H45" s="29" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B46" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G46" s="29" t="s">
+        <v>248</v>
+      </c>
+      <c r="H46" s="29" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B47" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G47" s="29" t="s">
+        <v>249</v>
+      </c>
+      <c r="H47" s="29" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B48" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G48" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="H48" s="29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B49" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G49" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="H49" s="29" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B50" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="F50" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="G50" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="H50" s="28" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B51" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="F51" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="G51" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="H51" s="28" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B52" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="F52" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="G52" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="H52" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="L13" s="28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B14" s="29" t="s">
-        <v>219</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>234</v>
-      </c>
-      <c r="H14" s="29" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B15" s="29" t="s">
-        <v>219</v>
-      </c>
-      <c r="G15" s="29" t="s">
-        <v>235</v>
-      </c>
-      <c r="H15" s="29" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B16" s="29" t="s">
-        <v>219</v>
-      </c>
-      <c r="G16" s="29" t="s">
-        <v>236</v>
-      </c>
-      <c r="H16" s="29" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="29" t="s">
-        <v>219</v>
-      </c>
-      <c r="G17" s="29" t="s">
-        <v>237</v>
-      </c>
-      <c r="H17" s="29" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="29" t="s">
-        <v>219</v>
-      </c>
-      <c r="G18" s="29" t="s">
-        <v>238</v>
-      </c>
-      <c r="H18" s="29" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="29" t="s">
-        <v>219</v>
-      </c>
-      <c r="G19" s="29" t="s">
-        <v>240</v>
-      </c>
-      <c r="H19" s="29" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="29" t="s">
-        <v>219</v>
-      </c>
-      <c r="G20" s="29" t="s">
-        <v>242</v>
-      </c>
-      <c r="H20" s="29" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="29" t="s">
+    </row>
+    <row r="53" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B53" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="F53" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="G53" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="H53" s="28" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B54" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="F54" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="G54" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="H54" s="28" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B55" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="F55" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="G55" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="H55" s="28" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B56" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="F56" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="G56" s="29" t="s">
         <v>220</v>
       </c>
-      <c r="G21" s="29" t="s">
-        <v>258</v>
-      </c>
-      <c r="H21" s="29" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="29" t="s">
+      <c r="H56" s="28" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B57" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="F57" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="G57" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="H57" s="28" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="B58" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="F58" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="G58" s="29" t="s">
         <v>220</v>
       </c>
-      <c r="G22" s="29" t="s">
-        <v>252</v>
-      </c>
-      <c r="H22" s="29" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G23" s="29" t="s">
-        <v>259</v>
-      </c>
-      <c r="H23" s="29" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G24" s="29" t="s">
-        <v>245</v>
-      </c>
-      <c r="H24" s="29" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G25" s="29" t="s">
-        <v>260</v>
-      </c>
-      <c r="H25" s="29" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G26" s="29" t="s">
-        <v>261</v>
-      </c>
-      <c r="H26" s="29" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G27" s="29" t="s">
-        <v>262</v>
-      </c>
-      <c r="H27" s="29" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G28" s="29" t="s">
-        <v>263</v>
-      </c>
-      <c r="H28" s="29" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G29" s="29" t="s">
-        <v>264</v>
-      </c>
-      <c r="H29" s="29" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G30" s="29" t="s">
-        <v>265</v>
-      </c>
-      <c r="H30" s="29" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G31" s="29" t="s">
-        <v>266</v>
-      </c>
-      <c r="H31" s="29" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G32" s="29" t="s">
-        <v>257</v>
-      </c>
-      <c r="H32" s="29" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G33" s="29" t="s">
-        <v>257</v>
-      </c>
-      <c r="H33" s="29" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G34" s="29" t="s">
-        <v>267</v>
-      </c>
-      <c r="H34" s="29" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G35" s="29" t="s">
-        <v>268</v>
-      </c>
-      <c r="H35" s="29" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G36" s="29" t="s">
-        <v>244</v>
-      </c>
-      <c r="H36" s="29" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G37" s="29" t="s">
-        <v>231</v>
-      </c>
-      <c r="H37" s="29" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G38" s="29" t="s">
-        <v>269</v>
-      </c>
-      <c r="H38" s="29" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G39" s="29" t="s">
-        <v>270</v>
-      </c>
-      <c r="H39" s="29" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G40" s="29" t="s">
-        <v>271</v>
-      </c>
-      <c r="H40" s="29" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G41" s="29" t="s">
-        <v>272</v>
-      </c>
-      <c r="H41" s="29" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G42" s="29" t="s">
-        <v>273</v>
-      </c>
-      <c r="H42" s="29" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G43" s="29" t="s">
-        <v>274</v>
-      </c>
-      <c r="H43" s="29" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G44" s="29" t="s">
-        <v>275</v>
-      </c>
-      <c r="H44" s="29" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G45" s="29" t="s">
-        <v>276</v>
-      </c>
-      <c r="H45" s="29" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G46" s="29" t="s">
-        <v>277</v>
-      </c>
-      <c r="H46" s="29" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G47" s="29" t="s">
-        <v>278</v>
-      </c>
-      <c r="H47" s="29" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G48" s="29" t="s">
-        <v>232</v>
-      </c>
-      <c r="H48" s="29" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G49" s="29" t="s">
-        <v>233</v>
-      </c>
-      <c r="H49" s="29" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="50" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="29" t="s">
-        <v>230</v>
-      </c>
-      <c r="F50" s="29" t="s">
-        <v>231</v>
-      </c>
-      <c r="G50" s="29" t="s">
-        <v>246</v>
-      </c>
-      <c r="H50" s="28" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="29" t="s">
-        <v>230</v>
-      </c>
-      <c r="F51" s="29" t="s">
-        <v>231</v>
-      </c>
-      <c r="G51" s="29" t="s">
-        <v>247</v>
-      </c>
-      <c r="H51" s="28" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="29" t="s">
-        <v>230</v>
-      </c>
-      <c r="F52" s="29" t="s">
-        <v>231</v>
-      </c>
-      <c r="G52" s="29" t="s">
-        <v>248</v>
-      </c>
-      <c r="H52" s="28" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="29" t="s">
-        <v>230</v>
-      </c>
-      <c r="F53" s="29" t="s">
-        <v>232</v>
-      </c>
-      <c r="G53" s="29" t="s">
-        <v>246</v>
-      </c>
-      <c r="H53" s="28" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="29" t="s">
-        <v>230</v>
-      </c>
-      <c r="F54" s="29" t="s">
-        <v>233</v>
-      </c>
-      <c r="G54" s="29" t="s">
-        <v>246</v>
-      </c>
-      <c r="H54" s="28" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="29" t="s">
-        <v>230</v>
-      </c>
-      <c r="F55" s="29" t="s">
-        <v>245</v>
-      </c>
-      <c r="G55" s="29" t="s">
-        <v>246</v>
-      </c>
-      <c r="H55" s="28" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="56" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="29" t="s">
-        <v>230</v>
-      </c>
-      <c r="F56" s="29" t="s">
-        <v>245</v>
-      </c>
-      <c r="G56" s="29" t="s">
-        <v>249</v>
-      </c>
-      <c r="H56" s="28" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="29" t="s">
-        <v>230</v>
-      </c>
-      <c r="F57" s="29" t="s">
-        <v>257</v>
-      </c>
-      <c r="G57" s="29" t="s">
-        <v>246</v>
-      </c>
-      <c r="H57" s="28" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="29" t="s">
-        <v>230</v>
-      </c>
-      <c r="F58" s="29" t="s">
-        <v>257</v>
-      </c>
-      <c r="G58" s="29" t="s">
-        <v>249</v>
-      </c>
       <c r="H58" s="28" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B59" s="29" t="s">
-        <v>221</v>
+        <v>192</v>
       </c>
       <c r="G59" s="28" t="s">
-        <v>164</v>
+        <v>330</v>
       </c>
       <c r="H59" s="28" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B60" s="29" t="s">
-        <v>221</v>
+        <v>192</v>
       </c>
       <c r="G60" s="28" t="s">
-        <v>165</v>
+        <v>331</v>
       </c>
       <c r="H60" s="28" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B61" s="29" t="s">
-        <v>221</v>
+        <v>192</v>
       </c>
       <c r="G61" s="28" t="s">
-        <v>166</v>
+        <v>332</v>
       </c>
       <c r="H61" s="28" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B62" s="29" t="s">
-        <v>221</v>
+        <v>192</v>
       </c>
       <c r="G62" s="28" t="s">
-        <v>167</v>
+        <v>333</v>
       </c>
       <c r="H62" s="28" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B63" s="29" t="s">
-        <v>221</v>
+        <v>192</v>
       </c>
       <c r="G63" s="28" t="s">
-        <v>168</v>
+        <v>334</v>
       </c>
       <c r="H63" s="28" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B64" s="29" t="s">
-        <v>221</v>
+        <v>192</v>
       </c>
       <c r="G64" s="28" t="s">
-        <v>169</v>
+        <v>335</v>
       </c>
       <c r="H64" s="28" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B65" s="29" t="s">
-        <v>221</v>
+        <v>192</v>
       </c>
       <c r="G65" s="28" t="s">
-        <v>173</v>
+        <v>336</v>
       </c>
       <c r="H65" s="28" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="I65" s="29"/>
       <c r="J65" s="29"/>
     </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B66" s="29" t="s">
-        <v>222</v>
+        <v>193</v>
       </c>
       <c r="G66" s="28" t="s">
-        <v>175</v>
+        <v>337</v>
       </c>
       <c r="H66" s="28" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="I66" s="29"/>
       <c r="J66" s="29"/>
     </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B67" s="29" t="s">
-        <v>222</v>
+        <v>193</v>
       </c>
       <c r="G67" s="28" t="s">
-        <v>177</v>
+        <v>338</v>
       </c>
       <c r="H67" s="28" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="I67" s="29"/>
       <c r="J67" s="29"/>
     </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B68" s="29" t="s">
-        <v>222</v>
+        <v>193</v>
       </c>
       <c r="G68" s="28" t="s">
-        <v>179</v>
+        <v>339</v>
       </c>
       <c r="H68" s="28" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="I68" s="29"/>
       <c r="J68" s="29"/>
     </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B69" s="29" t="s">
-        <v>222</v>
+        <v>193</v>
       </c>
       <c r="G69" s="28" t="s">
-        <v>181</v>
+        <v>340</v>
       </c>
       <c r="H69" s="28" t="s">
-        <v>182</v>
+        <v>159</v>
       </c>
       <c r="I69" s="29"/>
       <c r="J69" s="29"/>
     </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B70" s="29" t="s">
-        <v>222</v>
+        <v>193</v>
       </c>
       <c r="G70" s="28" t="s">
-        <v>183</v>
+        <v>341</v>
       </c>
       <c r="H70" s="28" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="I70" s="29"/>
       <c r="J70" s="29"/>
     </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B71" s="29" t="s">
-        <v>222</v>
+        <v>193</v>
       </c>
       <c r="G71" s="28" t="s">
-        <v>185</v>
+        <v>342</v>
       </c>
       <c r="H71" s="28" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="I71" s="29"/>
       <c r="J71" s="29"/>
     </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B72" s="29" t="s">
-        <v>222</v>
+        <v>193</v>
       </c>
       <c r="G72" s="28" t="s">
-        <v>187</v>
+        <v>343</v>
       </c>
       <c r="H72" s="28" t="s">
-        <v>188</v>
+        <v>162</v>
       </c>
       <c r="I72" s="29"/>
       <c r="J72" s="29"/>
     </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B73" s="29" t="s">
-        <v>222</v>
+        <v>193</v>
       </c>
       <c r="G73" s="28" t="s">
-        <v>189</v>
+        <v>344</v>
       </c>
       <c r="H73" s="28" t="s">
-        <v>190</v>
+        <v>163</v>
       </c>
       <c r="I73" s="29"/>
       <c r="J73" s="29"/>
     </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B74" s="29" t="s">
-        <v>222</v>
+        <v>193</v>
       </c>
       <c r="G74" s="28" t="s">
-        <v>191</v>
+        <v>345</v>
       </c>
       <c r="H74" s="28" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="I74" s="29"/>
       <c r="J74" s="29"/>
     </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B75" s="29" t="s">
-        <v>222</v>
+        <v>193</v>
       </c>
       <c r="G75" s="28" t="s">
-        <v>193</v>
+        <v>317</v>
       </c>
       <c r="H75" s="28" t="s">
-        <v>194</v>
+        <v>165</v>
       </c>
       <c r="I75" s="29"/>
       <c r="J75" s="29"/>
     </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B76" s="29" t="s">
-        <v>303</v>
+        <v>274</v>
       </c>
       <c r="G76" s="29" t="s">
-        <v>309</v>
+        <v>280</v>
       </c>
       <c r="H76" s="29" t="s">
-        <v>310</v>
+        <v>281</v>
       </c>
       <c r="I76" s="29"/>
       <c r="J76" s="29"/>
     </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B77" s="29" t="s">
-        <v>303</v>
+        <v>274</v>
       </c>
       <c r="G77" s="29" t="s">
-        <v>311</v>
+        <v>282</v>
       </c>
       <c r="H77" s="29" t="s">
-        <v>312</v>
+        <v>283</v>
       </c>
       <c r="I77" s="29"/>
       <c r="J77" s="29"/>
     </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B78" s="29" t="s">
-        <v>303</v>
+        <v>274</v>
       </c>
       <c r="G78" s="29" t="s">
-        <v>313</v>
+        <v>284</v>
       </c>
       <c r="H78" s="29" t="s">
-        <v>314</v>
+        <v>285</v>
       </c>
       <c r="I78" s="29"/>
       <c r="J78" s="29"/>
     </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B79" s="29" t="s">
-        <v>303</v>
+        <v>274</v>
       </c>
       <c r="G79" s="29" t="s">
-        <v>315</v>
+        <v>286</v>
       </c>
       <c r="H79" s="29" t="s">
-        <v>316</v>
+        <v>287</v>
       </c>
       <c r="I79" s="29"/>
       <c r="J79" s="29"/>
     </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B80" s="29" t="s">
-        <v>303</v>
+        <v>274</v>
       </c>
       <c r="G80" s="29" t="s">
-        <v>317</v>
+        <v>288</v>
       </c>
       <c r="H80" s="29" t="s">
-        <v>318</v>
+        <v>289</v>
       </c>
       <c r="I80" s="29"/>
       <c r="J80" s="29"/>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B81" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="G81" s="28" t="s">
+        <v>290</v>
+      </c>
+      <c r="H81" s="28" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B82" s="29" t="s">
+        <v>292</v>
+      </c>
+      <c r="G82" s="28" t="s">
+        <v>308</v>
+      </c>
+      <c r="H82" s="28" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B83" s="29" t="s">
+        <v>292</v>
+      </c>
+      <c r="G83" s="28" t="s">
+        <v>309</v>
+      </c>
+      <c r="H83" s="28" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B84" s="29" t="s">
+        <v>292</v>
+      </c>
+      <c r="G84" s="28" t="s">
+        <v>310</v>
+      </c>
+      <c r="H84" s="28" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B85" s="29" t="s">
+        <v>292</v>
+      </c>
+      <c r="G85" s="28" t="s">
+        <v>311</v>
+      </c>
+      <c r="H85" s="28" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B86" s="29" t="s">
+        <v>292</v>
+      </c>
+      <c r="G86" s="28" t="s">
+        <v>312</v>
+      </c>
+      <c r="H86" s="28" t="s">
         <v>303</v>
       </c>
-      <c r="G81" s="28" t="s">
-        <v>319</v>
-      </c>
-      <c r="H81" s="28" t="s">
-        <v>320</v>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B87" s="29" t="s">
+        <v>294</v>
+      </c>
+      <c r="G87" s="28" t="s">
+        <v>313</v>
+      </c>
+      <c r="H87" s="28" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B88" s="29" t="s">
+        <v>294</v>
+      </c>
+      <c r="G88" s="28" t="s">
+        <v>314</v>
+      </c>
+      <c r="H88" s="28" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B89" s="29" t="s">
+        <v>294</v>
+      </c>
+      <c r="G89" s="28" t="s">
+        <v>315</v>
+      </c>
+      <c r="H89" s="28" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B90" s="29" t="s">
+        <v>294</v>
+      </c>
+      <c r="G90" s="28" t="s">
+        <v>316</v>
+      </c>
+      <c r="H90" s="28" t="s">
+        <v>307</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:U1"/>
   <customSheetViews>
+    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+      <autoFilter ref="A1:U95065"/>
+    </customSheetView>
     <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" showAutoFilter="1" topLeftCell="D1">
       <pane ySplit="1" topLeftCell="A8937" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="F8956" sqref="F8956"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId1"/>
+      <pageSetup orientation="portrait" r:id="rId2"/>
       <autoFilter ref="A1:U88662"/>
-    </customSheetView>
-    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="A1:U95065"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4255,15 +4579,53 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="0fff5a07-2326-481b-a4e9-87ff7a79f8dd">Z7QZ4QWJDNQ7-73874190-25</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="0fff5a07-2326-481b-a4e9-87ff7a79f8dd">
-      <Url>https://jcp.sharepoint.com/sites/SPOProjects/JCPDotcomPortfolio/AssortmentExpansion/_layouts/15/DocIdRedir.aspx?ID=Z7QZ4QWJDNQ7-73874190-25</Url>
-      <Description>Z7QZ4QWJDNQ7-73874190-25</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4445,53 +4807,15 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="0fff5a07-2326-481b-a4e9-87ff7a79f8dd">Z7QZ4QWJDNQ7-73874190-25</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="0fff5a07-2326-481b-a4e9-87ff7a79f8dd">
+      <Url>https://jcp.sharepoint.com/sites/SPOProjects/JCPDotcomPortfolio/AssortmentExpansion/_layouts/15/DocIdRedir.aspx?ID=Z7QZ4QWJDNQ7-73874190-25</Url>
+      <Description>Z7QZ4QWJDNQ7-73874190-25</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4503,11 +4827,9 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{555FFCAF-FC77-46D2-BC80-D87BD036D3AD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D4AAD41-1536-4B20-8E6C-DCC51C90900F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0fff5a07-2326-481b-a4e9-87ff7a79f8dd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4532,9 +4854,11 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D4AAD41-1536-4B20-8E6C-DCC51C90900F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{555FFCAF-FC77-46D2-BC80-D87BD036D3AD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0fff5a07-2326-481b-a4e9-87ff7a79f8dd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added more attributes and reference data (** Ignore flag added, also added data types from MDM 7.6)
</commit_message>
<xml_diff>
--- a/seeddata-bsdf/99-exceldmd/PIM2.0v5 - Reference Data Model.xlsx
+++ b/seeddata-bsdf/99-exceldmd/PIM2.0v5 - Reference Data Model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="38325" windowHeight="23535" tabRatio="544"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="38325" windowHeight="23535" tabRatio="544" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="HELP" sheetId="1" r:id="rId1"/>
@@ -38,8 +38,8 @@
   </definedNames>
   <calcPr calcId="145621" iterateDelta="1E-4" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Gupta, Kunal - Personal View" guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1360" windowHeight="539" tabRatio="500" activeSheetId="7"/>
     <customWorkbookView name="Microsoft Office User - Personal View" guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1676" windowHeight="854" tabRatio="500" activeSheetId="7"/>
-    <customWorkbookView name="Gupta, Kunal - Personal View" guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1360" windowHeight="539" tabRatio="500" activeSheetId="7"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="412">
   <si>
     <t>ACTION</t>
   </si>
@@ -1135,6 +1135,198 @@
   </si>
   <si>
     <t>reference data key values, used to clearly define what is simply "data" and what is not (values starting with c are expected to be Contexts)</t>
+  </si>
+  <si>
+    <t>dboolean</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>dbooleangrey</t>
+  </si>
+  <si>
+    <t>Boolean Key</t>
+  </si>
+  <si>
+    <t>zb0</t>
+  </si>
+  <si>
+    <t>zb1</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>zbb</t>
+  </si>
+  <si>
+    <t>Undefined</t>
+  </si>
+  <si>
+    <t>Critical Key</t>
+  </si>
+  <si>
+    <t>dbenefitfilter</t>
+  </si>
+  <si>
+    <t>Benefit Filter</t>
+  </si>
+  <si>
+    <t>Benefit Filter Key</t>
+  </si>
+  <si>
+    <t>Benefit Filter Label</t>
+  </si>
+  <si>
+    <t>Anti dandruff</t>
+  </si>
+  <si>
+    <t>Deo protection</t>
+  </si>
+  <si>
+    <t>Firming</t>
+  </si>
+  <si>
+    <t>2 in 1</t>
+  </si>
+  <si>
+    <t>Intensive care</t>
+  </si>
+  <si>
+    <t>Moisturizing</t>
+  </si>
+  <si>
+    <t>Nourishing</t>
+  </si>
+  <si>
+    <t>Volumizing</t>
+  </si>
+  <si>
+    <t>Paraben-free</t>
+  </si>
+  <si>
+    <t>Aluminium-free</t>
+  </si>
+  <si>
+    <t>Oil-free</t>
+  </si>
+  <si>
+    <t>Without aerosol</t>
+  </si>
+  <si>
+    <t>100% Professional</t>
+  </si>
+  <si>
+    <t>1 active ingredient</t>
+  </si>
+  <si>
+    <t>1:1 Personal Consultation</t>
+  </si>
+  <si>
+    <t>NIVEA Scent</t>
+  </si>
+  <si>
+    <t>No Ethyl Alcohol</t>
+  </si>
+  <si>
+    <t>zbf01</t>
+  </si>
+  <si>
+    <t>zbf02</t>
+  </si>
+  <si>
+    <t>zbf03</t>
+  </si>
+  <si>
+    <t>zbf04</t>
+  </si>
+  <si>
+    <t>zbf05</t>
+  </si>
+  <si>
+    <t>zbf06</t>
+  </si>
+  <si>
+    <t>zbf07</t>
+  </si>
+  <si>
+    <t>zbf08</t>
+  </si>
+  <si>
+    <t>zbf09</t>
+  </si>
+  <si>
+    <t>zbf10</t>
+  </si>
+  <si>
+    <t>zbf11</t>
+  </si>
+  <si>
+    <t>zbf12</t>
+  </si>
+  <si>
+    <t>zbf13</t>
+  </si>
+  <si>
+    <t>zbf14</t>
+  </si>
+  <si>
+    <t>zbf15</t>
+  </si>
+  <si>
+    <t>zbf16</t>
+  </si>
+  <si>
+    <t>/~/images/mam/-120291-1.png</t>
+  </si>
+  <si>
+    <t>/~/images/mam/-120274-1.png</t>
+  </si>
+  <si>
+    <t>/~/images/mam/-120278-1.png</t>
+  </si>
+  <si>
+    <t>/~/images/mam/-120283-1.png</t>
+  </si>
+  <si>
+    <t>/~/images/mam/-120280-1.png</t>
+  </si>
+  <si>
+    <t>/~/images/mam/-120281-1.png</t>
+  </si>
+  <si>
+    <t>/~/images/mam/-120282-1.png</t>
+  </si>
+  <si>
+    <t>/~/images/mam/-120290-1.png</t>
+  </si>
+  <si>
+    <t>/~/images/mam/-169213-1.png</t>
+  </si>
+  <si>
+    <t>/~/images/mam/-150228-1.png</t>
+  </si>
+  <si>
+    <t>/~/images/mam/-150227-1.png</t>
+  </si>
+  <si>
+    <t>/~/images/mam/-150226-1.png</t>
+  </si>
+  <si>
+    <t>ficon</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>Benefit Filter Icon</t>
+  </si>
+  <si>
+    <t>zbf17</t>
   </si>
 </sst>
 </file>
@@ -1391,13 +1583,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Excel Built-in Normal" xfId="3"/>
@@ -1729,7 +1921,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
@@ -1744,55 +1936,55 @@
       <c r="A1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="34"/>
+      <c r="C1" s="35"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="33"/>
+      <c r="C2" s="34"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="33"/>
+      <c r="C3" s="34"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="33"/>
+      <c r="C4" s="34"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="33"/>
+      <c r="C5" s="34"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="33"/>
+      <c r="C6" s="34"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="32" t="s">
@@ -1972,11 +2164,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="150">
+    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="150">
       <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="150">
+    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="150">
       <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -1999,7 +2191,7 @@
   <dimension ref="A4:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2146,11 +2338,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="139">
+    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="139">
       <selection activeCell="E22" sqref="E22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="139">
+    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="139">
       <selection activeCell="E22" sqref="E22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -2163,21 +2355,21 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.25" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="27.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2191,98 +2383,122 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="29" t="s">
+        <v>350</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="29" t="s">
         <v>188</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" s="29" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>189</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>190</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>191</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C7" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>192</v>
-      </c>
-      <c r="C6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B7" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="C7" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="C9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>274</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C10" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>201</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="35" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="33" t="s">
         <v>292</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C12" s="29" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="29" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C13" s="29" t="s">
         <v>295</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C14" t="s">
+        <v>360</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1"/>
   <customSheetViews>
+    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="125" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:D1194"/>
+    </customSheetView>
     <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="125" showAutoFilter="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:D1194"/>
-    </customSheetView>
-    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="125" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="A1:D1194"/>
     </customSheetView>
@@ -2294,16 +2510,16 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.125" bestFit="1" customWidth="1"/>
@@ -2323,7 +2539,7 @@
     <col min="19" max="19" width="13.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2382,7 +2598,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B2" s="29" t="s">
         <v>194</v>
       </c>
@@ -2405,7 +2621,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>195</v>
       </c>
@@ -2428,7 +2644,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>196</v>
       </c>
@@ -2445,7 +2661,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>197</v>
       </c>
@@ -2462,7 +2678,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>198</v>
       </c>
@@ -2479,7 +2695,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>199</v>
       </c>
@@ -2496,56 +2712,73 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>276</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="8" spans="1:19" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="29" t="s">
+        <v>408</v>
+      </c>
+      <c r="C8" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="E8" t="s">
-        <v>99</v>
-      </c>
-      <c r="F8" t="s">
-        <v>278</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="E8" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>409</v>
+      </c>
+      <c r="G8" s="29" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C9" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E9" t="s">
         <v>99</v>
       </c>
       <c r="F9" t="s">
+        <v>278</v>
+      </c>
+      <c r="G9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>277</v>
+      </c>
+      <c r="C10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="F10" t="s">
         <v>279</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G10" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:S1"/>
   <customSheetViews>
+    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="93" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+      <autoFilter ref="A1:S35"/>
+    </customSheetView>
     <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="93" showAutoFilter="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
       <autoFilter ref="A1:S43"/>
-    </customSheetView>
-    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="93" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-      <autoFilter ref="A1:S35"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2564,7 +2797,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.125" customWidth="1"/>
     <col min="4" max="4" width="16.375" customWidth="1"/>
@@ -2608,7 +2841,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>200</v>
       </c>
@@ -2630,11 +2863,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="107">
+    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="107">
       <selection activeCell="G10" sqref="G10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="107">
+    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="107">
       <selection activeCell="G10" sqref="G10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -2647,16 +2880,16 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.875" customWidth="1"/>
     <col min="4" max="4" width="29.875" bestFit="1" customWidth="1"/>
@@ -2674,7 +2907,7 @@
     <col min="16" max="16" width="17.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2724,9 +2957,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>188</v>
+        <v>348</v>
       </c>
       <c r="D2" s="29" t="s">
         <v>194</v>
@@ -2740,7 +2973,7 @@
       <c r="I2" s="29"/>
       <c r="J2" s="29"/>
       <c r="K2" s="29" t="s">
-        <v>105</v>
+        <v>351</v>
       </c>
       <c r="L2" s="29"/>
       <c r="M2" s="29" t="s">
@@ -2752,9 +2985,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" s="29" t="s">
-        <v>188</v>
+        <v>348</v>
       </c>
       <c r="D3" s="29" t="s">
         <v>195</v>
@@ -2768,7 +3001,7 @@
       <c r="I3" s="29"/>
       <c r="J3" s="29"/>
       <c r="K3" s="29" t="s">
-        <v>104</v>
+        <v>349</v>
       </c>
       <c r="L3" s="29"/>
       <c r="M3" s="29" t="s">
@@ -2780,491 +3013,632 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>189</v>
+    <row r="4" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="29" t="s">
+        <v>350</v>
       </c>
       <c r="D4" s="29" t="s">
         <v>194</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="K4" t="s">
-        <v>105</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="K4" s="29" t="s">
+        <v>351</v>
+      </c>
+      <c r="M4" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="29" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="29" t="s">
-        <v>189</v>
+        <v>350</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>195</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="K5" t="s">
-        <v>104</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="K5" s="29" t="s">
+        <v>349</v>
+      </c>
+      <c r="M5" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5" s="29" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="29" t="s">
+        <v>358</v>
+      </c>
+      <c r="M6" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" s="29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="M7" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="P7" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>189</v>
       </c>
-      <c r="D6" s="29" t="s">
-        <v>196</v>
-      </c>
-      <c r="K6" t="s">
-        <v>121</v>
-      </c>
-      <c r="P6" s="29" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B7" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>197</v>
-      </c>
-      <c r="K7" t="s">
-        <v>117</v>
-      </c>
-      <c r="P7" s="29" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B8" s="29" t="s">
-        <v>189</v>
-      </c>
       <c r="D8" s="29" t="s">
-        <v>198</v>
+        <v>194</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
       </c>
       <c r="K8" t="s">
-        <v>118</v>
-      </c>
-      <c r="P8" s="29" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="M8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9" s="29" t="s">
         <v>189</v>
       </c>
       <c r="D9" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="G9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" t="s">
+        <v>104</v>
+      </c>
+      <c r="M9" t="s">
+        <v>30</v>
+      </c>
+      <c r="P9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>196</v>
+      </c>
+      <c r="K10" t="s">
+        <v>121</v>
+      </c>
+      <c r="P10" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="K11" t="s">
+        <v>117</v>
+      </c>
+      <c r="P11" s="29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="K12" t="s">
+        <v>118</v>
+      </c>
+      <c r="P12" s="29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="D13" s="29" t="s">
         <v>199</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K13" t="s">
         <v>120</v>
       </c>
-      <c r="P9" s="29" t="s">
+      <c r="P13" s="29" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B10" s="29" t="s">
+    <row r="14" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="29" t="s">
         <v>190</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>194</v>
-      </c>
-      <c r="F10" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10" s="29" t="s">
-        <v>173</v>
-      </c>
-      <c r="M10" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="P10" s="29" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B11" s="29" t="s">
-        <v>190</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>195</v>
-      </c>
-      <c r="G11" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="K11" s="29" t="s">
-        <v>174</v>
-      </c>
-      <c r="M11" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="P11" s="29" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>191</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>194</v>
-      </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B13" s="29" t="s">
-        <v>191</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>195</v>
-      </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>201</v>
       </c>
       <c r="D14" s="29" t="s">
         <v>194</v>
       </c>
-      <c r="E14" s="29"/>
       <c r="F14" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
       <c r="K14" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="L14" s="29"/>
+        <v>173</v>
+      </c>
       <c r="M14" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="N14" s="29"/>
-      <c r="O14" s="29"/>
       <c r="P14" s="29" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="29" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>195</v>
       </c>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
       <c r="G15" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
       <c r="K15" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="L15" s="29"/>
+        <v>174</v>
+      </c>
       <c r="M15" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="N15" s="29"/>
-      <c r="O15" s="29"/>
       <c r="P15" s="29" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B16" s="29" t="s">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>191</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="L16" s="29"/>
+      <c r="M16" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="N16" s="29"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>201</v>
       </c>
-      <c r="E16" s="29" t="s">
-        <v>200</v>
-      </c>
-      <c r="K16" t="s">
-        <v>139</v>
-      </c>
-      <c r="P16" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>192</v>
-      </c>
-      <c r="D17" s="29" t="s">
+      <c r="D18" s="29" t="s">
         <v>194</v>
       </c>
-      <c r="F17" t="s">
+      <c r="E18" s="29"/>
+      <c r="F18" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="K17" t="s">
-        <v>168</v>
-      </c>
-      <c r="M17" t="s">
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="P17" t="s">
+      <c r="N18" s="29"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="29" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="2:16" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B18" s="29" t="s">
-        <v>192</v>
-      </c>
-      <c r="D18" s="29" t="s">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="D19" s="29" t="s">
         <v>195</v>
       </c>
-      <c r="G18" t="s">
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="K18" t="s">
-        <v>169</v>
-      </c>
-      <c r="M18" t="s">
-        <v>30</v>
-      </c>
-      <c r="P18" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B19" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>194</v>
-      </c>
-      <c r="F19" s="29" t="s">
-        <v>30</v>
-      </c>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
       <c r="K19" s="29" t="s">
-        <v>170</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="L19" s="29"/>
       <c r="M19" s="29" t="s">
         <v>30</v>
       </c>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
       <c r="P19" s="29" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="D20" s="29" t="s">
-        <v>195</v>
-      </c>
-      <c r="G20" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="K20" s="29" t="s">
-        <v>171</v>
-      </c>
-      <c r="M20" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="P20" s="29" t="s">
-        <v>74</v>
+        <v>201</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="K20" t="s">
+        <v>139</v>
+      </c>
+      <c r="P20" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>274</v>
+        <v>192</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>276</v>
-      </c>
-      <c r="G21" t="s">
+        <v>194</v>
+      </c>
+      <c r="F21" t="s">
         <v>30</v>
       </c>
+      <c r="K21" t="s">
+        <v>168</v>
+      </c>
+      <c r="M21" t="s">
+        <v>30</v>
+      </c>
       <c r="P21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B22" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="G22" t="s">
+        <v>30</v>
+      </c>
+      <c r="K22" t="s">
+        <v>169</v>
+      </c>
+      <c r="M22" t="s">
+        <v>30</v>
+      </c>
+      <c r="P22" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>274</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>277</v>
-      </c>
-      <c r="F22" t="s">
-        <v>30</v>
-      </c>
-      <c r="P22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="29" t="s">
-        <v>292</v>
-      </c>
-      <c r="C23" s="29"/>
+        <v>193</v>
+      </c>
       <c r="D23" s="29" t="s">
         <v>194</v>
       </c>
-      <c r="E23" s="29"/>
       <c r="F23" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
       <c r="K23" s="29" t="s">
-        <v>296</v>
-      </c>
-      <c r="L23" s="29"/>
+        <v>170</v>
+      </c>
       <c r="M23" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="N23" s="29"/>
-      <c r="O23" s="29"/>
       <c r="P23" s="29" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="29" t="s">
-        <v>292</v>
-      </c>
-      <c r="C24" s="29"/>
+        <v>193</v>
+      </c>
       <c r="D24" s="29" t="s">
         <v>195</v>
       </c>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
       <c r="G24" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="29"/>
       <c r="K24" s="29" t="s">
-        <v>297</v>
-      </c>
-      <c r="L24" s="29"/>
+        <v>171</v>
+      </c>
       <c r="M24" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="N24" s="29"/>
-      <c r="O24" s="29"/>
       <c r="P24" s="29" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="29" t="s">
+      <c r="B25" t="s">
+        <v>274</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>277</v>
+      </c>
+      <c r="F25" t="s">
+        <v>30</v>
+      </c>
+      <c r="P25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>274</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>276</v>
+      </c>
+      <c r="G26" t="s">
+        <v>30</v>
+      </c>
+      <c r="P26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B27" s="29" t="s">
+        <v>292</v>
+      </c>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29" t="s">
+        <v>296</v>
+      </c>
+      <c r="L27" s="29"/>
+      <c r="M27" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="N27" s="29"/>
+      <c r="O27" s="29"/>
+      <c r="P27" s="29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B28" s="29" t="s">
+        <v>292</v>
+      </c>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29" t="s">
+        <v>297</v>
+      </c>
+      <c r="L28" s="29"/>
+      <c r="M28" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="N28" s="29"/>
+      <c r="O28" s="29"/>
+      <c r="P28" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B29" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29" t="s">
+      <c r="C29" s="29"/>
+      <c r="D29" s="29" t="s">
         <v>194</v>
       </c>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29" t="s">
+      <c r="E29" s="29"/>
+      <c r="F29" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29" t="s">
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29" t="s">
         <v>298</v>
       </c>
-      <c r="L25" s="29"/>
-      <c r="M25" s="29" t="s">
+      <c r="L29" s="29"/>
+      <c r="M29" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="N25" s="29"/>
-      <c r="O25" s="29"/>
-      <c r="P25" s="29" t="s">
+      <c r="N29" s="29"/>
+      <c r="O29" s="29"/>
+      <c r="P29" s="29" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="29" t="s">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B30" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29" t="s">
+      <c r="C30" s="29"/>
+      <c r="D30" s="29" t="s">
         <v>195</v>
       </c>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29" t="s">
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29" t="s">
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29" t="s">
         <v>299</v>
       </c>
-      <c r="L26" s="29"/>
-      <c r="M26" s="29" t="s">
+      <c r="L30" s="29"/>
+      <c r="M30" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="N26" s="29"/>
-      <c r="O26" s="29"/>
-      <c r="P26" s="29" t="s">
+      <c r="N30" s="29"/>
+      <c r="O30" s="29"/>
+      <c r="P30" s="29" t="s">
         <v>74</v>
       </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>359</v>
+      </c>
+      <c r="D31" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="G31" s="29"/>
+      <c r="K31" t="s">
+        <v>361</v>
+      </c>
+      <c r="M31" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="P31" s="29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B32" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="K32" t="s">
+        <v>362</v>
+      </c>
+      <c r="M32" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="P32" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B33" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="D33" t="s">
+        <v>408</v>
+      </c>
+      <c r="K33" t="s">
+        <v>410</v>
+      </c>
+      <c r="P33" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D34" s="29"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:P1"/>
@@ -3272,19 +3646,19 @@
     <sortCondition ref="B1"/>
   </sortState>
   <customSheetViews>
+    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="90" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+      <autoFilter ref="A1:P2390"/>
+    </customSheetView>
     <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="90" showAutoFilter="1">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId1"/>
+      <pageSetup orientation="portrait" r:id="rId2"/>
       <autoFilter ref="A1:P2402"/>
-    </customSheetView>
-    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="90" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="A1:P2390"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3295,24 +3669,24 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:U90"/>
+  <dimension ref="A1:U112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.25" style="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.625" style="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.875" style="29" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.625" style="29" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.625" style="29" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.125" style="28" customWidth="1"/>
-    <col min="8" max="8" width="35.625" style="28" customWidth="1"/>
-    <col min="9" max="9" width="23.5" style="28" customWidth="1"/>
+    <col min="7" max="7" width="19.125" style="28" customWidth="1"/>
+    <col min="8" max="8" width="26.875" style="28" customWidth="1"/>
+    <col min="9" max="9" width="27" style="28" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.625" style="28" customWidth="1"/>
     <col min="11" max="11" width="68.375" style="29" customWidth="1"/>
     <col min="12" max="12" width="31.625" style="29" customWidth="1"/>
@@ -3323,7 +3697,7 @@
     <col min="22" max="16384" width="11" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3388,152 +3762,92 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B2" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>352</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B3" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B4" s="29" t="s">
+        <v>350</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>356</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B5" s="29" t="s">
+        <v>350</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>352</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B6" s="29" t="s">
+        <v>350</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B7" s="29" t="s">
         <v>188</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G7" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H7" s="28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B8" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>319</v>
+      </c>
+      <c r="H8" s="28" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B3" s="29" t="s">
-        <v>188</v>
-      </c>
-      <c r="G3" s="28" t="s">
-        <v>319</v>
-      </c>
-      <c r="H3" s="28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B4" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="G4" s="28" t="s">
-        <v>320</v>
-      </c>
-      <c r="H4" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="I4" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="J4" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="K4" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="L4" s="28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B5" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="G5" s="28" t="s">
-        <v>321</v>
-      </c>
-      <c r="H5" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="I5" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="J5" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="K5" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="L5" s="28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B6" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="G6" s="28" t="s">
-        <v>322</v>
-      </c>
-      <c r="H6" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="I6" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="J6" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="K6" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="L6" s="28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B7" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="G7" s="28" t="s">
-        <v>323</v>
-      </c>
-      <c r="H7" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="I7" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="J7" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="K7" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="L7" s="28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B8" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="G8" s="28" t="s">
-        <v>324</v>
-      </c>
-      <c r="H8" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="I8" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="J8" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="K8" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="L8" s="28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9" s="29" t="s">
         <v>189</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I9" s="28" t="s">
         <v>125</v>
@@ -3548,15 +3862,15 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B10" s="29" t="s">
         <v>189</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="I10" s="28" t="s">
         <v>125</v>
@@ -3571,15 +3885,15 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B11" s="29" t="s">
         <v>189</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="I11" s="28" t="s">
         <v>125</v>
@@ -3594,15 +3908,15 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B12" s="29" t="s">
         <v>189</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="H12" s="28" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I12" s="28" t="s">
         <v>125</v>
@@ -3617,15 +3931,15 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B13" s="29" t="s">
         <v>189</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="H13" s="28" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="I13" s="28" t="s">
         <v>125</v>
@@ -3640,478 +3954,571 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B14" s="29" t="s">
-        <v>190</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>205</v>
-      </c>
-      <c r="H14" s="29" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="I14" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="J14" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="K14" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="L14" s="28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B15" s="29" t="s">
-        <v>190</v>
-      </c>
-      <c r="G15" s="29" t="s">
-        <v>206</v>
-      </c>
-      <c r="H15" s="29" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" ht="15.95" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+      <c r="G15" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="H15" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="I15" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="J15" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="K15" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="L15" s="28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B16" s="29" t="s">
-        <v>190</v>
-      </c>
-      <c r="G16" s="29" t="s">
-        <v>207</v>
-      </c>
-      <c r="H16" s="29" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="15.95" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>327</v>
+      </c>
+      <c r="H16" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="I16" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="J16" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="K16" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="L16" s="28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="29" t="s">
-        <v>190</v>
-      </c>
-      <c r="G17" s="29" t="s">
-        <v>208</v>
-      </c>
-      <c r="H17" s="29" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="15.95" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+      <c r="G17" s="28" t="s">
+        <v>328</v>
+      </c>
+      <c r="H17" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="I17" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="J17" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="L17" s="28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="29" t="s">
-        <v>190</v>
-      </c>
-      <c r="G18" s="29" t="s">
-        <v>209</v>
-      </c>
-      <c r="H18" s="29" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="15.95" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+      <c r="G18" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="I18" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="J18" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="K18" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="L18" s="28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="29" t="s">
         <v>190</v>
       </c>
       <c r="G19" s="29" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="H19" s="29" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="15.95" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="29" t="s">
         <v>190</v>
       </c>
       <c r="G20" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="H20" s="29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="G21" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="H21" s="29" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="G22" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="H22" s="29" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="G23" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="H23" s="29" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="G24" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="H24" s="29" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="G25" s="29" t="s">
         <v>213</v>
       </c>
-      <c r="H20" s="29" t="s">
+      <c r="H25" s="29" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B21" s="29" t="s">
-        <v>191</v>
-      </c>
-      <c r="G21" s="29" t="s">
-        <v>229</v>
-      </c>
-      <c r="H21" s="29" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B22" s="29" t="s">
-        <v>191</v>
-      </c>
-      <c r="G22" s="29" t="s">
-        <v>223</v>
-      </c>
-      <c r="H22" s="29" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B23" s="29" t="s">
-        <v>191</v>
-      </c>
-      <c r="G23" s="29" t="s">
-        <v>230</v>
-      </c>
-      <c r="H23" s="29" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B24" s="29" t="s">
-        <v>191</v>
-      </c>
-      <c r="G24" s="29" t="s">
-        <v>216</v>
-      </c>
-      <c r="H24" s="29" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B25" s="29" t="s">
-        <v>191</v>
-      </c>
-      <c r="G25" s="29" t="s">
-        <v>231</v>
-      </c>
-      <c r="H25" s="29" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="29" t="s">
         <v>191</v>
       </c>
       <c r="G26" s="29" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H26" s="29" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="29" t="s">
         <v>191</v>
       </c>
       <c r="G27" s="29" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="H27" s="29" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="29" t="s">
         <v>191</v>
       </c>
       <c r="G28" s="29" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="H28" s="29" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="29" t="s">
         <v>191</v>
       </c>
       <c r="G29" s="29" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="H29" s="29" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="29" t="s">
         <v>191</v>
       </c>
       <c r="G30" s="29" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="H30" s="29" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="29" t="s">
         <v>191</v>
       </c>
       <c r="G31" s="29" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="H31" s="29" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="29" t="s">
         <v>191</v>
       </c>
       <c r="G32" s="29" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="H32" s="29" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+      <c r="I32" s="29"/>
+      <c r="J32" s="29"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="29" t="s">
         <v>191</v>
       </c>
       <c r="G33" s="29" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="H33" s="29" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="29" t="s">
         <v>191</v>
       </c>
       <c r="G34" s="29" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H34" s="29" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="29" t="s">
         <v>191</v>
       </c>
       <c r="G35" s="29" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="H35" s="29" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+      <c r="I35" s="29"/>
+      <c r="J35" s="29"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="29" t="s">
         <v>191</v>
       </c>
       <c r="G36" s="29" t="s">
-        <v>215</v>
+        <v>237</v>
       </c>
       <c r="H36" s="29" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="I36" s="29"/>
+      <c r="J36" s="29"/>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="29" t="s">
         <v>191</v>
       </c>
       <c r="G37" s="29" t="s">
-        <v>202</v>
+        <v>228</v>
       </c>
       <c r="H37" s="29" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+      <c r="I37" s="29"/>
+      <c r="J37" s="29"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="29" t="s">
         <v>191</v>
       </c>
       <c r="G38" s="29" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="H38" s="29" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="29" t="s">
         <v>191</v>
       </c>
       <c r="G39" s="29" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H39" s="29" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+      <c r="I39" s="29"/>
+      <c r="J39" s="29"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="29" t="s">
         <v>191</v>
       </c>
       <c r="G40" s="29" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H40" s="29" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="29" t="s">
         <v>191</v>
       </c>
       <c r="G41" s="29" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
       <c r="H41" s="29" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="I41" s="29"/>
+      <c r="J41" s="29"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="29" t="s">
         <v>191</v>
       </c>
       <c r="G42" s="29" t="s">
-        <v>244</v>
+        <v>202</v>
       </c>
       <c r="H42" s="29" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="I42" s="29"/>
+      <c r="J42" s="29"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="29" t="s">
         <v>191</v>
       </c>
       <c r="G43" s="29" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="H43" s="29" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="29" t="s">
         <v>191</v>
       </c>
       <c r="G44" s="29" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H44" s="29" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="29" t="s">
         <v>191</v>
       </c>
       <c r="G45" s="29" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="H45" s="29" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+      <c r="I45" s="29"/>
+      <c r="J45" s="29"/>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="29" t="s">
         <v>191</v>
       </c>
       <c r="G46" s="29" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="H46" s="29" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+      <c r="I46" s="29"/>
+      <c r="J46" s="29"/>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="29" t="s">
         <v>191</v>
       </c>
       <c r="G47" s="29" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="H47" s="29" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+      <c r="I47" s="29"/>
+      <c r="J47" s="29"/>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="29" t="s">
         <v>191</v>
       </c>
       <c r="G48" s="29" t="s">
-        <v>203</v>
+        <v>245</v>
       </c>
       <c r="H48" s="29" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+      <c r="I48" s="29"/>
+      <c r="J48" s="29"/>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" s="29" t="s">
         <v>191</v>
       </c>
       <c r="G49" s="29" t="s">
+        <v>246</v>
+      </c>
+      <c r="H49" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="I49" s="29"/>
+      <c r="J49" s="29"/>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B50" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G50" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="H50" s="29" t="s">
+        <v>270</v>
+      </c>
+      <c r="I50" s="29"/>
+      <c r="J50" s="29"/>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B51" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G51" s="29" t="s">
+        <v>248</v>
+      </c>
+      <c r="H51" s="29" t="s">
+        <v>271</v>
+      </c>
+      <c r="I51" s="29"/>
+      <c r="J51" s="29"/>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B52" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G52" s="29" t="s">
+        <v>249</v>
+      </c>
+      <c r="H52" s="29" t="s">
+        <v>272</v>
+      </c>
+      <c r="I52" s="29"/>
+      <c r="J52" s="29"/>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B53" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G53" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="H53" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="I53" s="29"/>
+      <c r="J53" s="29"/>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B54" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="G54" s="29" t="s">
         <v>204</v>
       </c>
-      <c r="H49" s="29" t="s">
+      <c r="H54" s="29" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="50" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B50" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="F50" s="29" t="s">
-        <v>202</v>
-      </c>
-      <c r="G50" s="29" t="s">
-        <v>217</v>
-      </c>
-      <c r="H50" s="28" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B51" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="F51" s="29" t="s">
-        <v>202</v>
-      </c>
-      <c r="G51" s="29" t="s">
-        <v>218</v>
-      </c>
-      <c r="H51" s="28" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B52" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="F52" s="29" t="s">
-        <v>202</v>
-      </c>
-      <c r="G52" s="29" t="s">
-        <v>219</v>
-      </c>
-      <c r="H52" s="28" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B53" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="F53" s="29" t="s">
-        <v>203</v>
-      </c>
-      <c r="G53" s="29" t="s">
-        <v>217</v>
-      </c>
-      <c r="H53" s="28" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B54" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="F54" s="29" t="s">
-        <v>204</v>
-      </c>
-      <c r="G54" s="29" t="s">
-        <v>217</v>
-      </c>
-      <c r="H54" s="28" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="I54" s="29"/>
+      <c r="J54" s="29"/>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B55" s="29" t="s">
         <v>201</v>
       </c>
       <c r="F55" s="29" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="G55" s="29" t="s">
         <v>217</v>
@@ -4119,189 +4526,224 @@
       <c r="H55" s="28" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="56" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="I55" s="29"/>
+      <c r="J55" s="29"/>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B56" s="29" t="s">
         <v>201</v>
       </c>
       <c r="F56" s="29" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="G56" s="29" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H56" s="28" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="I56" s="29"/>
+      <c r="J56" s="29"/>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B57" s="29" t="s">
         <v>201</v>
       </c>
       <c r="F57" s="29" t="s">
-        <v>228</v>
+        <v>202</v>
       </c>
       <c r="G57" s="29" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="H57" s="28" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="I57" s="29"/>
+      <c r="J57" s="29"/>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B58" s="29" t="s">
         <v>201</v>
       </c>
       <c r="F58" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="G58" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="H58" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="I58" s="29"/>
+      <c r="J58" s="29"/>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B59" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="F59" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="G59" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="H59" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="I59" s="29"/>
+      <c r="J59" s="29"/>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B60" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="F60" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="G60" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="H60" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="I60" s="29"/>
+      <c r="J60" s="29"/>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B61" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="F61" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="G61" s="29" t="s">
+        <v>220</v>
+      </c>
+      <c r="H61" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="I61" s="29"/>
+      <c r="J61" s="29"/>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B62" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="F62" s="29" t="s">
         <v>228</v>
       </c>
-      <c r="G58" s="29" t="s">
+      <c r="G62" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="H62" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="I62" s="29"/>
+      <c r="J62" s="29"/>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B63" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="F63" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="G63" s="29" t="s">
         <v>220</v>
       </c>
-      <c r="H58" s="28" t="s">
+      <c r="H63" s="28" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="59" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B59" s="29" t="s">
-        <v>192</v>
-      </c>
-      <c r="G59" s="28" t="s">
-        <v>330</v>
-      </c>
-      <c r="H59" s="28" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B60" s="29" t="s">
-        <v>192</v>
-      </c>
-      <c r="G60" s="28" t="s">
-        <v>331</v>
-      </c>
-      <c r="H60" s="28" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B61" s="29" t="s">
-        <v>192</v>
-      </c>
-      <c r="G61" s="28" t="s">
-        <v>332</v>
-      </c>
-      <c r="H61" s="28" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B62" s="29" t="s">
-        <v>192</v>
-      </c>
-      <c r="G62" s="28" t="s">
-        <v>333</v>
-      </c>
-      <c r="H62" s="28" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
-      <c r="B63" s="29" t="s">
-        <v>192</v>
-      </c>
-      <c r="G63" s="28" t="s">
-        <v>334</v>
-      </c>
-      <c r="H63" s="28" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8" s="29" customFormat="1" ht="15.95" x14ac:dyDescent="0.25">
+      <c r="I63" s="29"/>
+      <c r="J63" s="29"/>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B64" s="29" t="s">
         <v>192</v>
       </c>
       <c r="G64" s="28" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="H64" s="28" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="65" spans="2:10" ht="15.95" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="I64" s="29"/>
+      <c r="J64" s="29"/>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B65" s="29" t="s">
         <v>192</v>
       </c>
       <c r="G65" s="28" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="H65" s="28" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I65" s="29"/>
       <c r="J65" s="29"/>
     </row>
-    <row r="66" spans="2:10" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B66" s="29" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G66" s="28" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="H66" s="28" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I66" s="29"/>
       <c r="J66" s="29"/>
     </row>
-    <row r="67" spans="2:10" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B67" s="29" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G67" s="28" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="H67" s="28" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="I67" s="29"/>
       <c r="J67" s="29"/>
     </row>
-    <row r="68" spans="2:10" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B68" s="29" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G68" s="28" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="H68" s="28" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="I68" s="29"/>
       <c r="J68" s="29"/>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B69" s="29" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G69" s="28" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="H69" s="28" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="I69" s="29"/>
       <c r="J69" s="29"/>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B70" s="29" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G70" s="28" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="H70" s="28" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="I70" s="29"/>
       <c r="J70" s="29"/>
@@ -4311,10 +4753,10 @@
         <v>193</v>
       </c>
       <c r="G71" s="28" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="H71" s="28" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="I71" s="29"/>
       <c r="J71" s="29"/>
@@ -4324,10 +4766,10 @@
         <v>193</v>
       </c>
       <c r="G72" s="28" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="H72" s="28" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="I72" s="29"/>
       <c r="J72" s="29"/>
@@ -4337,10 +4779,10 @@
         <v>193</v>
       </c>
       <c r="G73" s="28" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="H73" s="28" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="I73" s="29"/>
       <c r="J73" s="29"/>
@@ -4350,10 +4792,10 @@
         <v>193</v>
       </c>
       <c r="G74" s="28" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="H74" s="28" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="I74" s="29"/>
       <c r="J74" s="29"/>
@@ -4363,205 +4805,508 @@
         <v>193</v>
       </c>
       <c r="G75" s="28" t="s">
-        <v>317</v>
+        <v>341</v>
       </c>
       <c r="H75" s="28" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="I75" s="29"/>
       <c r="J75" s="29"/>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B76" s="29" t="s">
-        <v>274</v>
-      </c>
-      <c r="G76" s="29" t="s">
-        <v>280</v>
-      </c>
-      <c r="H76" s="29" t="s">
-        <v>281</v>
+        <v>193</v>
+      </c>
+      <c r="G76" s="28" t="s">
+        <v>342</v>
+      </c>
+      <c r="H76" s="28" t="s">
+        <v>161</v>
       </c>
       <c r="I76" s="29"/>
       <c r="J76" s="29"/>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B77" s="29" t="s">
-        <v>274</v>
-      </c>
-      <c r="G77" s="29" t="s">
-        <v>282</v>
-      </c>
-      <c r="H77" s="29" t="s">
-        <v>283</v>
+        <v>193</v>
+      </c>
+      <c r="G77" s="28" t="s">
+        <v>343</v>
+      </c>
+      <c r="H77" s="28" t="s">
+        <v>162</v>
       </c>
       <c r="I77" s="29"/>
       <c r="J77" s="29"/>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B78" s="29" t="s">
-        <v>274</v>
-      </c>
-      <c r="G78" s="29" t="s">
-        <v>284</v>
-      </c>
-      <c r="H78" s="29" t="s">
-        <v>285</v>
+        <v>193</v>
+      </c>
+      <c r="G78" s="28" t="s">
+        <v>344</v>
+      </c>
+      <c r="H78" s="28" t="s">
+        <v>163</v>
       </c>
       <c r="I78" s="29"/>
       <c r="J78" s="29"/>
     </row>
     <row r="79" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B79" s="29" t="s">
-        <v>274</v>
-      </c>
-      <c r="G79" s="29" t="s">
-        <v>286</v>
-      </c>
-      <c r="H79" s="29" t="s">
-        <v>287</v>
+        <v>193</v>
+      </c>
+      <c r="G79" s="28" t="s">
+        <v>345</v>
+      </c>
+      <c r="H79" s="28" t="s">
+        <v>164</v>
       </c>
       <c r="I79" s="29"/>
       <c r="J79" s="29"/>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B80" s="29" t="s">
-        <v>274</v>
-      </c>
-      <c r="G80" s="29" t="s">
-        <v>288</v>
-      </c>
-      <c r="H80" s="29" t="s">
-        <v>289</v>
+        <v>193</v>
+      </c>
+      <c r="G80" s="28" t="s">
+        <v>317</v>
+      </c>
+      <c r="H80" s="28" t="s">
+        <v>165</v>
       </c>
       <c r="I80" s="29"/>
       <c r="J80" s="29"/>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B81" s="29" t="s">
         <v>274</v>
       </c>
-      <c r="G81" s="28" t="s">
+      <c r="G81" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="H81" s="29" t="s">
+        <v>281</v>
+      </c>
+      <c r="I81" s="29"/>
+      <c r="J81" s="29"/>
+    </row>
+    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B82" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="G82" s="29" t="s">
+        <v>282</v>
+      </c>
+      <c r="H82" s="29" t="s">
+        <v>283</v>
+      </c>
+      <c r="I82" s="29"/>
+      <c r="J82" s="29"/>
+    </row>
+    <row r="83" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B83" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="G83" s="29" t="s">
+        <v>284</v>
+      </c>
+      <c r="H83" s="29" t="s">
+        <v>285</v>
+      </c>
+      <c r="I83" s="29"/>
+      <c r="J83" s="29"/>
+    </row>
+    <row r="84" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B84" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="G84" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="H84" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="I84" s="29"/>
+      <c r="J84" s="29"/>
+    </row>
+    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B85" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="G85" s="29" t="s">
+        <v>288</v>
+      </c>
+      <c r="H85" s="29" t="s">
+        <v>289</v>
+      </c>
+      <c r="I85" s="29"/>
+      <c r="J85" s="29"/>
+    </row>
+    <row r="86" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B86" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="G86" s="28" t="s">
         <v>290</v>
       </c>
-      <c r="H81" s="28" t="s">
+      <c r="H86" s="28" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B82" s="29" t="s">
+    <row r="87" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B87" s="29" t="s">
         <v>292</v>
       </c>
-      <c r="G82" s="28" t="s">
+      <c r="G87" s="28" t="s">
         <v>308</v>
       </c>
-      <c r="H82" s="28" t="s">
+      <c r="H87" s="28" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B83" s="29" t="s">
+    <row r="88" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B88" s="29" t="s">
         <v>292</v>
       </c>
-      <c r="G83" s="28" t="s">
+      <c r="G88" s="28" t="s">
         <v>309</v>
       </c>
-      <c r="H83" s="28" t="s">
+      <c r="H88" s="28" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B84" s="29" t="s">
+    <row r="89" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B89" s="29" t="s">
         <v>292</v>
       </c>
-      <c r="G84" s="28" t="s">
+      <c r="G89" s="28" t="s">
         <v>310</v>
       </c>
-      <c r="H84" s="28" t="s">
+      <c r="H89" s="28" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B85" s="29" t="s">
+    <row r="90" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B90" s="29" t="s">
         <v>292</v>
       </c>
-      <c r="G85" s="28" t="s">
+      <c r="G90" s="28" t="s">
         <v>311</v>
       </c>
-      <c r="H85" s="28" t="s">
+      <c r="H90" s="28" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B86" s="29" t="s">
+    <row r="91" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B91" s="29" t="s">
         <v>292</v>
       </c>
-      <c r="G86" s="28" t="s">
+      <c r="G91" s="28" t="s">
         <v>312</v>
       </c>
-      <c r="H86" s="28" t="s">
+      <c r="H91" s="28" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B87" s="29" t="s">
+    <row r="92" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B92" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="G87" s="28" t="s">
+      <c r="G92" s="28" t="s">
         <v>313</v>
       </c>
-      <c r="H87" s="28" t="s">
+      <c r="H92" s="28" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B88" s="29" t="s">
+    <row r="93" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B93" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="G88" s="28" t="s">
+      <c r="G93" s="28" t="s">
         <v>314</v>
       </c>
-      <c r="H88" s="28" t="s">
+      <c r="H93" s="28" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B89" s="29" t="s">
+    <row r="94" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B94" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="G89" s="28" t="s">
+      <c r="G94" s="28" t="s">
         <v>315</v>
       </c>
-      <c r="H89" s="28" t="s">
+      <c r="H94" s="28" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B90" s="29" t="s">
+    <row r="95" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B95" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="G90" s="28" t="s">
+      <c r="G95" s="28" t="s">
         <v>316</v>
       </c>
-      <c r="H90" s="28" t="s">
+      <c r="H95" s="28" t="s">
         <v>307</v>
+      </c>
+    </row>
+    <row r="96" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B96" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="G96" s="28" t="s">
+        <v>380</v>
+      </c>
+      <c r="H96" s="28" t="s">
+        <v>363</v>
+      </c>
+      <c r="I96" s="28" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B97" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="G97" s="28" t="s">
+        <v>381</v>
+      </c>
+      <c r="H97" s="28" t="s">
+        <v>364</v>
+      </c>
+      <c r="I97" s="28" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B98" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="G98" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="H98" s="28" t="s">
+        <v>365</v>
+      </c>
+      <c r="I98" s="28" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B99" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="G99" s="28" t="s">
+        <v>383</v>
+      </c>
+      <c r="H99" s="28" t="s">
+        <v>366</v>
+      </c>
+      <c r="I99" s="28" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B100" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="G100" s="28" t="s">
+        <v>384</v>
+      </c>
+      <c r="H100" s="28" t="s">
+        <v>367</v>
+      </c>
+      <c r="I100" s="28" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B101" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="G101" s="28" t="s">
+        <v>385</v>
+      </c>
+      <c r="H101" s="28" t="s">
+        <v>368</v>
+      </c>
+      <c r="I101" s="28" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B102" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="G102" s="28" t="s">
+        <v>386</v>
+      </c>
+      <c r="H102" s="28" t="s">
+        <v>369</v>
+      </c>
+      <c r="I102" s="28" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B103" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="G103" s="28" t="s">
+        <v>387</v>
+      </c>
+      <c r="H103" s="28" t="s">
+        <v>370</v>
+      </c>
+      <c r="I103" s="28" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B104" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="G104" s="28" t="s">
+        <v>388</v>
+      </c>
+      <c r="H104" s="28" t="s">
+        <v>371</v>
+      </c>
+      <c r="I104" s="28" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B105" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="G105" s="28" t="s">
+        <v>389</v>
+      </c>
+      <c r="H105" s="28" t="s">
+        <v>372</v>
+      </c>
+      <c r="I105" s="28" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B106" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="G106" s="28" t="s">
+        <v>390</v>
+      </c>
+      <c r="H106" s="28" t="s">
+        <v>373</v>
+      </c>
+      <c r="I106" s="28" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B107" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="G107" s="28" t="s">
+        <v>391</v>
+      </c>
+      <c r="H107" s="28" t="s">
+        <v>374</v>
+      </c>
+      <c r="I107" s="28" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B108" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="G108" s="28" t="s">
+        <v>392</v>
+      </c>
+      <c r="H108" s="28" t="s">
+        <v>375</v>
+      </c>
+      <c r="I108" s="28" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B109" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="G109" s="28" t="s">
+        <v>393</v>
+      </c>
+      <c r="H109" s="28" t="s">
+        <v>376</v>
+      </c>
+      <c r="I109" s="28" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B110" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="G110" s="28" t="s">
+        <v>394</v>
+      </c>
+      <c r="H110" s="28" t="s">
+        <v>377</v>
+      </c>
+      <c r="I110" s="28" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B111" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="G111" s="28" t="s">
+        <v>395</v>
+      </c>
+      <c r="H111" s="28" t="s">
+        <v>378</v>
+      </c>
+      <c r="I111" s="28" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B112" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="G112" s="28" t="s">
+        <v>411</v>
+      </c>
+      <c r="H112" s="28" t="s">
+        <v>379</v>
+      </c>
+      <c r="I112" s="28" t="s">
+        <v>404</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:U1"/>
   <customSheetViews>
+    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" showAutoFilter="1" topLeftCell="D1">
+      <pane ySplit="1" topLeftCell="A8937" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="F8956" sqref="F8956"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+      <autoFilter ref="A1:U88662"/>
+    </customSheetView>
     <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" showAutoFilter="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId1"/>
+      <pageSetup orientation="portrait" r:id="rId2"/>
       <autoFilter ref="A1:U95065"/>
-    </customSheetView>
-    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" showAutoFilter="1" topLeftCell="D1">
-      <pane ySplit="1" topLeftCell="A8937" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F8956" sqref="F8956"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="A1:U88662"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4579,53 +5324,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="0fff5a07-2326-481b-a4e9-87ff7a79f8dd">Z7QZ4QWJDNQ7-73874190-25</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="0fff5a07-2326-481b-a4e9-87ff7a79f8dd">
+      <Url>https://jcp.sharepoint.com/sites/SPOProjects/JCPDotcomPortfolio/AssortmentExpansion/_layouts/15/DocIdRedir.aspx?ID=Z7QZ4QWJDNQ7-73874190-25</Url>
+      <Description>Z7QZ4QWJDNQ7-73874190-25</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4807,15 +5514,53 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="0fff5a07-2326-481b-a4e9-87ff7a79f8dd">Z7QZ4QWJDNQ7-73874190-25</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="0fff5a07-2326-481b-a4e9-87ff7a79f8dd">
-      <Url>https://jcp.sharepoint.com/sites/SPOProjects/JCPDotcomPortfolio/AssortmentExpansion/_layouts/15/DocIdRedir.aspx?ID=Z7QZ4QWJDNQ7-73874190-25</Url>
-      <Description>Z7QZ4QWJDNQ7-73874190-25</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4827,9 +5572,11 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D4AAD41-1536-4B20-8E6C-DCC51C90900F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{555FFCAF-FC77-46D2-BC80-D87BD036D3AD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0fff5a07-2326-481b-a4e9-87ff7a79f8dd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4854,11 +5601,9 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{555FFCAF-FC77-46D2-BC80-D87BD036D3AD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D4AAD41-1536-4B20-8E6C-DCC51C90900F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0fff5a07-2326-481b-a4e9-87ff7a79f8dd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updates to bsdf model and configs
</commit_message>
<xml_diff>
--- a/seeddata-bsdf/99-exceldmd/PIM2.0v5 - Reference Data Model.xlsx
+++ b/seeddata-bsdf/99-exceldmd/PIM2.0v5 - Reference Data Model.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\a\git\Beiersdorf\seeddata-bsdf\99-exceldmd\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikhilbhatia/github/Beiersdorf/seeddata-bsdf/99-exceldmd/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="38325" windowHeight="23535" tabRatio="544" activeTab="6"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="38320" windowHeight="23540" tabRatio="544" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="HELP" sheetId="1" r:id="rId1"/>
@@ -38,8 +38,8 @@
   </definedNames>
   <calcPr calcId="145621" iterateDelta="1E-4" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1676" windowHeight="854" tabRatio="500" activeSheetId="7"/>
     <customWorkbookView name="Gupta, Kunal - Personal View" guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1360" windowHeight="539" tabRatio="500" activeSheetId="7"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1676" windowHeight="854" tabRatio="500" activeSheetId="7"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -58,7 +58,7 @@
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1332,7 +1332,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]General"/>
   </numFmts>
@@ -1918,18 +1918,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.125" customWidth="1"/>
-    <col min="3" max="3" width="90.625" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" customWidth="1"/>
+    <col min="3" max="3" width="90.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2164,11 +2164,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="150">
+    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="150">
       <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="150">
+    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="150">
       <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -2187,21 +2187,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2"/>
+  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A4:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2338,11 +2338,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="139">
+    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="139">
       <selection activeCell="E22" sqref="E22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="139">
+    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="139">
       <selection activeCell="E22" sqref="E22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -2354,7 +2354,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet3"/>
+  <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2362,10 +2362,10 @@
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="27.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2490,15 +2490,15 @@
   </sheetData>
   <autoFilter ref="A1:D1"/>
   <customSheetViews>
+    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="125" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:D1194"/>
+    </customSheetView>
     <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="125" showAutoFilter="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:D1194"/>
-    </customSheetView>
-    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="125" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="A1:D1194"/>
     </customSheetView>
@@ -2509,7 +2509,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet4"/>
+  <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2517,26 +2517,26 @@
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -2766,19 +2766,19 @@
   </sheetData>
   <autoFilter ref="A1:S1"/>
   <customSheetViews>
+    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="93" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+      <autoFilter ref="A1:S43"/>
+    </customSheetView>
     <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="93" showAutoFilter="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
       <autoFilter ref="A1:S35"/>
-    </customSheetView>
-    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="93" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-      <autoFilter ref="A1:S43"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2788,28 +2788,28 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet5"/>
+  <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.125" customWidth="1"/>
-    <col min="4" max="4" width="16.375" customWidth="1"/>
-    <col min="5" max="5" width="16.625" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="10" customWidth="1"/>
-    <col min="7" max="7" width="15.125" customWidth="1"/>
-    <col min="8" max="8" width="16.625" customWidth="1"/>
-    <col min="9" max="9" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2863,11 +2863,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="107">
+    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="107">
       <selection activeCell="G10" sqref="G10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="107">
+    <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="107">
       <selection activeCell="G10" sqref="G10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -2879,7 +2879,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet6"/>
+  <sheetPr codeName="Sheet6" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2887,24 +2887,24 @@
       <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.875" customWidth="1"/>
-    <col min="4" max="4" width="29.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" customWidth="1"/>
+    <col min="4" max="4" width="29.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.5" customWidth="1"/>
-    <col min="7" max="7" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.625" customWidth="1"/>
-    <col min="10" max="10" width="21.875" customWidth="1"/>
-    <col min="11" max="11" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.375" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" customWidth="1"/>
+    <col min="10" max="10" width="21.83203125" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" customWidth="1"/>
     <col min="13" max="13" width="17.5" customWidth="1"/>
-    <col min="14" max="14" width="19.125" customWidth="1"/>
+    <col min="14" max="14" width="19.1640625" customWidth="1"/>
     <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -3646,19 +3646,19 @@
     <sortCondition ref="B1"/>
   </sortState>
   <customSheetViews>
+    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="90" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+      <autoFilter ref="A1:P2402"/>
+    </customSheetView>
     <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" scale="90" showAutoFilter="1">
       <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId1"/>
+      <pageSetup orientation="portrait" r:id="rId2"/>
       <autoFilter ref="A1:P2390"/>
-    </customSheetView>
-    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" scale="90" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="A1:P2402"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3668,31 +3668,31 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet7"/>
+  <sheetPr codeName="Sheet7" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A113" sqref="A113"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.25" style="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.625" style="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.875" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.625" style="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.625" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="29" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.125" style="28" customWidth="1"/>
-    <col min="8" max="8" width="26.875" style="28" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" style="28" customWidth="1"/>
+    <col min="8" max="8" width="26.83203125" style="28" customWidth="1"/>
     <col min="9" max="9" width="27" style="28" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.625" style="28" customWidth="1"/>
-    <col min="11" max="11" width="68.375" style="29" customWidth="1"/>
-    <col min="12" max="12" width="31.625" style="29" customWidth="1"/>
-    <col min="13" max="15" width="14.125" style="29" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.125" style="29" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.125" style="29" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" style="28" customWidth="1"/>
+    <col min="11" max="11" width="68.33203125" style="29" customWidth="1"/>
+    <col min="12" max="12" width="31.6640625" style="29" customWidth="1"/>
+    <col min="13" max="15" width="14.1640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.1640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.1640625" style="29" bestFit="1" customWidth="1"/>
     <col min="18" max="21" width="17" style="29" bestFit="1" customWidth="1"/>
     <col min="22" max="16384" width="11" style="29"/>
   </cols>
@@ -5294,19 +5294,19 @@
   </sheetData>
   <autoFilter ref="A1:U1"/>
   <customSheetViews>
+    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+      <autoFilter ref="A1:U95065"/>
+    </customSheetView>
     <customSheetView guid="{7B5BF384-6D74-4070-814F-9CC686E1DAC3}" showAutoFilter="1" topLeftCell="D1">
       <pane ySplit="1" topLeftCell="A8937" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="F8956" sqref="F8956"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId1"/>
+      <pageSetup orientation="portrait" r:id="rId2"/>
       <autoFilter ref="A1:U88662"/>
-    </customSheetView>
-    <customSheetView guid="{F370B4E9-6EF8-7A46-9C9D-1B3D4A45BDBB}" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="A1:U95065"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5316,6 +5316,56 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
@@ -5323,7 +5373,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_dlc_DocId xmlns="0fff5a07-2326-481b-a4e9-87ff7a79f8dd">Z7QZ4QWJDNQ7-73874190-25</_dlc_DocId>
@@ -5335,7 +5385,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003CF273DB610BE64D8338C714685CCF46" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2352d1590348b4df6d1de565ccbd102a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fff5a07-2326-481b-a4e9-87ff7a79f8dd" xmlns:ns3="2e2046eb-f52d-433a-aad8-97c651e3992c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5c0a0cba47b5c64de8255dd546e4ec9" ns2:_="" ns3:_="">
     <xsd:import namespace="0fff5a07-2326-481b-a4e9-87ff7a79f8dd"/>
@@ -5513,57 +5563,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D4AAD41-1536-4B20-8E6C-DCC51C90900F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB6AEA0-3DF2-4494-BDE5-510837701A22}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -5571,7 +5579,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{555FFCAF-FC77-46D2-BC80-D87BD036D3AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -5581,7 +5589,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50D230FB-949A-4A81-A3AC-DBDE1CC696FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5598,12 +5606,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D4AAD41-1536-4B20-8E6C-DCC51C90900F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>